<commit_message>
Update coding sheet. Add P3's pre diary data
</commit_message>
<xml_diff>
--- a/assignmentSubmissions/assignment7_coding/coding.xlsx
+++ b/assignmentSubmissions/assignment7_coding/coding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burak-inofab/git/ModelingUX/assignmentSubmissions/assignment7_coding/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abura\git\ModelingUX\assignmentSubmissions\assignment7_coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406EEA0D-F4E5-844A-A571-C91C2D3307F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F37D26C-3B9F-4350-824F-B2E06BCA9930}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="3260" windowWidth="25600" windowHeight="15540" xr2:uid="{F4C71E44-69F0-DC4C-BDEB-22E2A60C66CE}"/>
+    <workbookView xWindow="6405" yWindow="3255" windowWidth="25605" windowHeight="15540" xr2:uid="{F4C71E44-69F0-DC4C-BDEB-22E2A60C66CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Coding" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="114">
   <si>
     <t>Code</t>
   </si>
@@ -155,48 +155,6 @@
     <t>P5</t>
   </si>
   <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>P12</t>
-  </si>
-  <si>
-    <t>P13</t>
-  </si>
-  <si>
-    <t>P14</t>
-  </si>
-  <si>
-    <t>P15</t>
-  </si>
-  <si>
-    <t>P16</t>
-  </si>
-  <si>
-    <t>P17</t>
-  </si>
-  <si>
-    <t>P18</t>
-  </si>
-  <si>
-    <t>P19</t>
-  </si>
-  <si>
     <t>Hanefi Gürler</t>
   </si>
   <si>
@@ -309,6 +267,111 @@
   </si>
   <si>
     <t>ders yok</t>
+  </si>
+  <si>
+    <t>6 sene boyunca aşı tedavisi gördüm ve bu süreçte alerjik neler beni etkiliyor bunlardan korunmayı öğrendim ki hala sağlıklı kalmak adına yaptığım en büyük şey bu alerjenlerden uzak durmak.</t>
+  </si>
+  <si>
+    <t>Ilaç kullanmama sonrası kötü deneyim</t>
+  </si>
+  <si>
+    <t>Kötü deneyim sonrası düzenli ilaç kullanma</t>
+  </si>
+  <si>
+    <t>Aileden hatırlatma desteği</t>
+  </si>
+  <si>
+    <t>İlaçları göz önünde tutma</t>
+  </si>
+  <si>
+    <t>Bir kere kullanmadığında alışkanlık kaybı yaşama</t>
+  </si>
+  <si>
+    <t>Büyüdükçe vücut değişiyor. Etrafındaki alerjenler de değişyor. Buraya geldikten sonra özellikle polen konusunda çok sıkıntı çektim. Nefesim falan sıkışıyordu.</t>
+  </si>
+  <si>
+    <t>Çevre şartlarının değişiminin hastalığa kötü etkisi</t>
+  </si>
+  <si>
+    <t>Bir şeye sürekli muhtaç kalmak çok kötü bir şey</t>
+  </si>
+  <si>
+    <t>Aynı zamanda beni bir yerlere götürmüyor, hatta bazı yerlerimi tembelleştiriyor gibi hissettiriyordu</t>
+  </si>
+  <si>
+    <t>Hatta fanusun içinde büyüdüm gibi geliyor annem evde dikkat ederdi her şeye simdi ben dikkat ediyorum</t>
+  </si>
+  <si>
+    <t>Öyle olunca kullandım bir süre daha sonra sıkıntım yok diye tekrar ilaç kullanmayı bıraktım</t>
+  </si>
+  <si>
+    <t>İki sene boyunca inhaler kullanmaya devam ettim ama sonrasında böyle şey bir yerden sonra devam etmesi çok zor. çok yorucu bir şey. Bir şekilde kalıyor ya da aksıyor.</t>
+  </si>
+  <si>
+    <t>İlaç kullanıyor olmanın kötü hissettirmesi</t>
+  </si>
+  <si>
+    <t>Aileden hastalığa karşı korunma yardımı</t>
+  </si>
+  <si>
+    <t>İyi hissettiği için ilaç kullanmayı kesmek</t>
+  </si>
+  <si>
+    <t>İlaç kullanmayı bıraktıktan sonra solunum sıkıntılarım artmaya başladı</t>
+  </si>
+  <si>
+    <t>Sürekli hasta ve aciz hissediyordum kendimi. Hasta olmanın getirdiği bir acizlik hissi var.</t>
+  </si>
+  <si>
+    <t>Tedaviye başladıktan sonra her şey bir süre çok iyi gitti. Alerjenlerden korunduktan sonra gerçekten hasta olmuyordum. Hayatımda hiç olmadığım kadar sağlıklı hissettim. 8 sene falan iyi hissettim.</t>
+  </si>
+  <si>
+    <t>Sigara dumanından korunmaya çalışmak büyük bir sıkıntı oldu hep benim için.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astıma bakış açım giderek kötüleşti. Başta o kadar büyük bir sorun olarak görmüyordum. Ama tekrar 7 yaşımda kullandığım ilaçları kullanmaya başlayınca baya ağladığımı hatırlıyorum. </t>
+  </si>
+  <si>
+    <t>Astımın bitmediğini hep biliyordum ama tedavinin hiçbir işe yaramayıp sıfıra dönmesi kötü oldu.</t>
+  </si>
+  <si>
+    <t>İyileşemedin aslında hep zayıfsın, hastalıktan bağımsız da zayıfsın gibi geldi. Semptom olsa da olmasa da.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sürekli kullanman gereken bir şey ve çok da bir sonuç elde edemediğin bir şey o yüzden hayat boyu ona bağımlı kalmış olmak da hoş değil.</t>
+  </si>
+  <si>
+    <t>Bağımlı kaldığımı hissettiğim anda ilaç kullanmayı bırakmak istedim. Sonrasında sadece kötü olduğum zamanlarda destekleyici ile kullanmaya başladım. Çok doğru bir şey değil ama.</t>
+  </si>
+  <si>
+    <t>Normalde İzmitliyim orası daha nemli. Oraya döndüğümde daha kötü oluyorum. 1 ay falan da geçmiyor hastalığım. Bir daha ne zaman olacağım diye bekliyordum açıkçası</t>
+  </si>
+  <si>
+    <t>Zayıflık algısı bağımlılık hissi gibi psikolojik şeyleri zamanla biraz atlattım. Tamam bu bir hastalık, bunu yaşayan başka insanlar da var. Bu kişilik vs gibi konularda senin zayıf olduğun anlamına gelmiyor. Tamam bir ilaca muhtaçsın ama bu herkesin başına gelebilecek bir durum, farklı insanların da başına gelebiliyor.</t>
+  </si>
+  <si>
+    <t>Çok fazla şeye dikkat ediyordum. Dışardasın arkadaşlarınlasın mesela, işte senin şunu yapmaman lazım senin şunu yememen lazım buna alerjin var. Şunu yapmaman lazım bronşlarını şeyapar.</t>
+  </si>
+  <si>
+    <t>Arı sokmaması lazım mesala en büyük korkum hala. Ona da alerjim var. Bronşlarımı şişiriyormuş.</t>
+  </si>
+  <si>
+    <t>İnsanlar eğleniyorlar bir şeyler yapıyorlar mesela sigaralı ortam en büyük kabusum. Dahil olamıyorum, bir şeylerde hep bir eksik kalıyordum dolayısı ile bu bir zayıflık gibi geliyordu.</t>
+  </si>
+  <si>
+    <t>Rahatsızlanmam sonrası 1bucuk aydır tekrar düzenli ilaç kullanmaya başladım</t>
+  </si>
+  <si>
+    <t>Arada atladığım oluyor ilaç kullanmayı. Sabahları aceleyle çıkarken unutuyorum bazen ama akşamları genelde hatırlıyorum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kesinlikle gözümün önünde olan bir yere koyuyorum. Yurtta bu daha kolaydı zaten bir tane masa var kesin biliyorum sabah ve akşam oraya bakacağımı. </t>
+  </si>
+  <si>
+    <t>Çizelge yapıyordum . Yaptım yaptım diye işaretliyordum. Sonunda bir ödül yoktu ama çizelgede check ediyordum.</t>
+  </si>
+  <si>
+    <t>Derslerle ilgili olabilir onemli hayatımdaki diğer seylerle ilgili ya da edinemediğim ama edinmek istediğim alışkanlıklarda da çizelge yapıyorum. Mesela su ıcme icin yapıyorum her gun su içme alışkanlığı için</t>
   </si>
 </sst>
 </file>
@@ -819,19 +882,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353ADEC9-000A-354D-8FBD-32DD4E097B7B}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="118" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="114.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="88.375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.375" customWidth="1"/>
+    <col min="5" max="5" width="27.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -845,7 +909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -859,7 +923,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -873,7 +937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -886,8 +950,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -900,8 +967,11 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -914,8 +984,11 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -928,8 +1001,11 @@
       <c r="D7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -942,8 +1018,11 @@
       <c r="D8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -957,7 +1036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -970,8 +1049,11 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -985,7 +1067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -999,7 +1081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1013,7 +1095,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1027,7 +1109,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1041,7 +1123,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1055,7 +1137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1069,7 +1151,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1083,7 +1165,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1097,7 +1179,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1111,7 +1193,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1125,7 +1207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1139,7 +1221,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1153,7 +1235,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1167,7 +1249,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1181,7 +1263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1195,7 +1277,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1203,284 +1285,634 @@
         <v>35</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
         <v>35</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B30" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>35</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>35</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="D34" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>35</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>35</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D38" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D40" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B41" t="s">
         <v>35</v>
       </c>
       <c r="C41" s="15" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D41" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
         <v>35</v>
       </c>
       <c r="C42" s="15" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B43" t="s">
         <v>35</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D43" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="B45" t="s">
         <v>35</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>36</v>
+      </c>
       <c r="B46" t="s">
         <v>35</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D46" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="64" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
       <c r="B47" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>38</v>
+      </c>
+      <c r="B48" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D47" t="s">
-        <v>7</v>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>38</v>
+      </c>
+      <c r="B49" t="s">
+        <v>33</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+      <c r="E49" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>38</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>38</v>
+      </c>
+      <c r="B51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>38</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>38</v>
+      </c>
+      <c r="B55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>38</v>
+      </c>
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>38</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>38</v>
+      </c>
+      <c r="B58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+      <c r="B59" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>38</v>
+      </c>
+      <c r="B61" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>38</v>
+      </c>
+      <c r="B62" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>38</v>
+      </c>
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>38</v>
+      </c>
+      <c r="B65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>38</v>
+      </c>
+      <c r="B66" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B67" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>38</v>
+      </c>
+      <c r="B69" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>38</v>
+      </c>
+      <c r="B70" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B71" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>38</v>
+      </c>
+      <c r="B73" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>38</v>
+      </c>
+      <c r="B75" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1522,46 +1954,46 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1574,34 +2006,34 @@
   <dimension ref="A1:AU9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="3" max="47" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.375" customWidth="1"/>
+    <col min="3" max="47" width="3.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:47" ht="17" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="AL2" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="AS2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" ht="17" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C3" s="7">
         <v>26</v>
@@ -1739,144 +2171,144 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="F4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="G4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="J4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="K4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="L4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="M4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="N4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="P4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="Q4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="R4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="S4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="T4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="U4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="W4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="X4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="Y4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="Z4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="AA4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="AB4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="AC4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="AD4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="AE4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="AF4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="AG4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="AH4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="AI4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="AJ4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="AK4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="AL4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="AM4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="AN4" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="AO4" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="AP4" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="AQ4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="AR4" s="10" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="AS4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="AT4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="AU4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>36</v>
       </c>
@@ -1889,29 +2321,36 @@
       <c r="I5" s="4"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>37</v>
       </c>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>38</v>
       </c>
       <c r="Q7" s="5"/>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="AA7" s="6"/>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>39</v>
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>40</v>
       </c>
-      <c r="Y9" s="5"/>
+      <c r="AE9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Work on coding. Add 2 more people and halfway done with categorization
</commit_message>
<xml_diff>
--- a/assignmentSubmissions/assignment7_coding/coding.xlsx
+++ b/assignmentSubmissions/assignment7_coding/coding.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abura\git\ModelingUX\assignmentSubmissions\assignment7_coding\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burak-inofab/git/ModelingUX/assignmentSubmissions/assignment7_coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F37D26C-3B9F-4350-824F-B2E06BCA9930}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A86B2B-1E3F-FF41-9FE4-D8B63B65B965}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="3255" windowWidth="25605" windowHeight="15540" xr2:uid="{F4C71E44-69F0-DC4C-BDEB-22E2A60C66CE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{F4C71E44-69F0-DC4C-BDEB-22E2A60C66CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Coding" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Calendar" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coding!$A$1:$D$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coding!$A$1:$F$106</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="193">
   <si>
     <t>Code</t>
   </si>
@@ -272,27 +272,9 @@
     <t>6 sene boyunca aşı tedavisi gördüm ve bu süreçte alerjik neler beni etkiliyor bunlardan korunmayı öğrendim ki hala sağlıklı kalmak adına yaptığım en büyük şey bu alerjenlerden uzak durmak.</t>
   </si>
   <si>
-    <t>Ilaç kullanmama sonrası kötü deneyim</t>
-  </si>
-  <si>
-    <t>Kötü deneyim sonrası düzenli ilaç kullanma</t>
-  </si>
-  <si>
-    <t>Aileden hatırlatma desteği</t>
-  </si>
-  <si>
-    <t>İlaçları göz önünde tutma</t>
-  </si>
-  <si>
-    <t>Bir kere kullanmadığında alışkanlık kaybı yaşama</t>
-  </si>
-  <si>
     <t>Büyüdükçe vücut değişiyor. Etrafındaki alerjenler de değişyor. Buraya geldikten sonra özellikle polen konusunda çok sıkıntı çektim. Nefesim falan sıkışıyordu.</t>
   </si>
   <si>
-    <t>Çevre şartlarının değişiminin hastalığa kötü etkisi</t>
-  </si>
-  <si>
     <t>Bir şeye sürekli muhtaç kalmak çok kötü bir şey</t>
   </si>
   <si>
@@ -308,15 +290,6 @@
     <t>İki sene boyunca inhaler kullanmaya devam ettim ama sonrasında böyle şey bir yerden sonra devam etmesi çok zor. çok yorucu bir şey. Bir şekilde kalıyor ya da aksıyor.</t>
   </si>
   <si>
-    <t>İlaç kullanıyor olmanın kötü hissettirmesi</t>
-  </si>
-  <si>
-    <t>Aileden hastalığa karşı korunma yardımı</t>
-  </si>
-  <si>
-    <t>İyi hissettiği için ilaç kullanmayı kesmek</t>
-  </si>
-  <si>
     <t>İlaç kullanmayı bıraktıktan sonra solunum sıkıntılarım artmaya başladı</t>
   </si>
   <si>
@@ -372,6 +345,270 @@
   </si>
   <si>
     <t>Derslerle ilgili olabilir onemli hayatımdaki diğer seylerle ilgili ya da edinemediğim ama edinmek istediğim alışkanlıklarda da çizelge yapıyorum. Mesela su ıcme icin yapıyorum her gun su içme alışkanlığı için</t>
+  </si>
+  <si>
+    <t>Yanıma almayı düşünmedim yani aklıma gelmedi, unuttum sayılabilir.</t>
+  </si>
+  <si>
+    <t>İlacımı bir kere kullanmamak, sürekli kullanmayacağımı daha çok pekiştiriyor bir yada birkaç kere aksaması. Arada kopcak zaten diye düşünüyorum. O zaman daha rahat bırakıyorum kullanmayı.</t>
+  </si>
+  <si>
+    <t>Çarşamba gecesi uyumadım, perşembeye paper yetiştiriyordum. Uyumayınca aklıma gelmedi hiç.</t>
+  </si>
+  <si>
+    <t>Kullansam da kullanmasam da tamamen iyileşmeyeceğim, ama daha iyi bir durumda olacağımı bildiğim için ilacımı kullanıyorum</t>
+  </si>
+  <si>
+    <t>Küçükken nefesim tıkanıyordu, beşikteyken duvarlara vuruyordum. Acil e gidiyorduk bu durumda.</t>
+  </si>
+  <si>
+    <t>Sonrasında eve buhar makinesi aldık acile gitmemeye başladık.</t>
+  </si>
+  <si>
+    <t>Doktor bana şehir değiştir, sen burada yaşamayazsın dedi.</t>
+  </si>
+  <si>
+    <t>Bir iki sene ilaç kullandım ve yaşamım normale döndü.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adana biraz daha sıcak ve çok nemli. Öyle ortamlarda nefes almam çok zor oluyor. Yazın 60 derece 50 derece hissedilen sıcaklık olduğundan nefes almak baya zorlaşıyor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kortizonlu ilaçlar kilo yapıyor ve çok faza yan etkisi var. </t>
+  </si>
+  <si>
+    <t>Benim de şey gibi bir rahatsızlığım yoktu yani her an ilaç kullanmam gerektiği şekilde değildi yani o yüzden de bi yerden sonra doktorun söylemesinden çok kendi bildiğimi okuyup o şekilde bir yol çizdim.</t>
+  </si>
+  <si>
+    <t>Ventolin uyurken ya da normal zamanda titreme yapıyor. Annem dişimn sesine uyanıyordu geceleri.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arkadaşlar dışarda bir şeyler yapıyor, ben durmak zorundayım çünkü dışarı çıkarsam tıkanıyorum. </t>
+  </si>
+  <si>
+    <t>Fiziksel etkilerin yanında sosyal çevremi de çok etkiledi.</t>
+  </si>
+  <si>
+    <t>Kortizonlu ilaçlar çarpıntı yapıyor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Küçük olduğumdan babam ilaçlarımı takip ederdi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Babamda da astım vardı, eve özel temizleyici kokusuz şeyler almışlardı. </t>
+  </si>
+  <si>
+    <t>Özel sağlık sigortam bitti, doktora bir kere daha gidebildim 500-600 tl para vererek, bu sefer de baktık böyle devam edemeyeceğiz. Biraz da Türk mantığıyla: bu ilaçları kullanınca sıkıntı olmadığını farkettik ve dedik ki biz bunları kullanmaya devam edelim.</t>
+  </si>
+  <si>
+    <t>Uzun bir süre sonra, Lise 2 gibiydi, tekrar doktora gittim ve bana dedi ki senin bu ilaçları bırakman gerekiyor. Bunu bu kadar uzun süre kullanmamalıydın. Bunu çok önceden bırakman gerekiyordu dedi. Niye daha önce gelmediniz diye kızdı.</t>
+  </si>
+  <si>
+    <t>Orada düzeni bozmamızdaki sebep biraz maddiyat oldu.</t>
+  </si>
+  <si>
+    <t>Grip olduğum zaman ciğerlerime iniyor ve nefes alamıyorum.</t>
+  </si>
+  <si>
+    <t>Raporum bitmiş, raporu burada çıkartamadığımdan 50-60 tl civarı bir para verdim ilaçlar için.</t>
+  </si>
+  <si>
+    <t>Doğdumdan beri bu durum olduğundan artık kend kendimin doktoru olmak gibi gereksiz özgüvenli bir hareket oluyor.</t>
+  </si>
+  <si>
+    <t>Hasta olduğumda ben gidişatı genelde biliyorum. Doğru olan şey aslında pratikte sıkıntılı geliyor. Onları kendi kendime toplamaya çalıştım. Ona göre kendime böyle bir yol çizdim. O yüzden şu an sadece atak halinde bunu kullanıyorum.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yanımda biri sigara içse dumanından direk iptal olan bir insandım ama bunlar için tedavi oldum. Şu an için düzenli olarak ilaç kullanmam gerektiğini düşünmüyorum. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astım bir yere kadar iyileşiyor, tamamen iyileşme gibi bir durum söz konusu değil. Şu an hayatımdan memnunum açıkçası. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 günlükken bir morarmışım ilk, apar topar hastaneye kaldırmışlar. Kafamdan serum vermişler. Ondan sonra 4-5 yaşlarımda Astım teşhisi kondu. </t>
+  </si>
+  <si>
+    <t>Babam beni gece uyandırıp bir seans buhar makinesi ile ilaç verirdi.</t>
+  </si>
+  <si>
+    <t>Doktor durumumun iyi olduğunu söyledi, ilaçları ben de biraz azalttım, sonrasında ise kötü oldum. Merdiven çıkmaydı, top oynama vs çok tıkanıyordum. Duruyordum böyle bir yerde nefes alamıyordum.</t>
+  </si>
+  <si>
+    <t>Üniversiteye geldikten sonra tamamen kestim ilaçları. Bir kere artık o kadar top oynamamaya başladım.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arada halı sahaya giderken cebimde ventolin götürüp kalenin yanına koyuyorum. </t>
+  </si>
+  <si>
+    <t>Yine yoruluyorum falan tabi hızlı yürüdüğümde vs ama tabi o lisedeki kadar kesilme yaşamıyorum.</t>
+  </si>
+  <si>
+    <t>İlaç kullandığım süre boyunca ilk başlarda hiçbir şey değişmedi, sonradan değişti.</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Missing one dose negatively affected adherence behavior</t>
+  </si>
+  <si>
+    <t>Got sick of using medication</t>
+  </si>
+  <si>
+    <t>Bad memory</t>
+  </si>
+  <si>
+    <t>Drop out reason</t>
+  </si>
+  <si>
+    <t>Lived in hospital for a month when 10 years old</t>
+  </si>
+  <si>
+    <t>Experienced excarbation after dropping out using medicine</t>
+  </si>
+  <si>
+    <t>Started using medicine again after a bad incident</t>
+  </si>
+  <si>
+    <t>Motivation for using medicine</t>
+  </si>
+  <si>
+    <t>Family support</t>
+  </si>
+  <si>
+    <t>Mother reminded medicine time</t>
+  </si>
+  <si>
+    <t>Mother set up a routine: use medicine before sitting on breakfast table</t>
+  </si>
+  <si>
+    <t>Reason for missing a dose</t>
+  </si>
+  <si>
+    <t>Breaking the routine affects adherence negatively</t>
+  </si>
+  <si>
+    <t>Strategy to build-up adherence</t>
+  </si>
+  <si>
+    <t>Storing medicine in a visible spot helps reminding</t>
+  </si>
+  <si>
+    <t>During hospitalization, strict schedule of medication use helped him gaining the habit</t>
+  </si>
+  <si>
+    <t>Wake up routine change affects adherence negatively</t>
+  </si>
+  <si>
+    <t>Not seeing the positive or negative impact directly affects adherence motivation negatively</t>
+  </si>
+  <si>
+    <t>Prior experience of negative consequences helps motivate adherence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Using a pill box to organize all the medication help avoid skipping doses </t>
+  </si>
+  <si>
+    <t>Using a pill box helps when you are mobile</t>
+  </si>
+  <si>
+    <t>Snoozing mobile app notification leads to missed dose</t>
+  </si>
+  <si>
+    <t>Breaking the routine (being tired) affects adherence negatively</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missed a dose while rushing </t>
+  </si>
+  <si>
+    <t>Ideal drug reminder</t>
+  </si>
+  <si>
+    <t>When near by the drug, something should warn to take it</t>
+  </si>
+  <si>
+    <t>Breaking the routine (sleeping in somwehere else) affects adherence negatively</t>
+  </si>
+  <si>
+    <t>Ran out of drugs because they were not visible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breaking the routine (sleeping in somwehere else) affects adherence negatively, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">It is hard to spare time to get prescription &amp; pick up the drugs </t>
+  </si>
+  <si>
+    <t>Pharmacies do not always have the meds in stock so multiple visits required</t>
+  </si>
+  <si>
+    <t>Wrong diagnosis statement entered to system causes social security not to rebate</t>
+  </si>
+  <si>
+    <t>When ran out of drugs, missed some doses until buying new ones</t>
+  </si>
+  <si>
+    <t>Ran out of some drugs earlier than it is stated on the packaging</t>
+  </si>
+  <si>
+    <t>Keeping away from alergens since childhood</t>
+  </si>
+  <si>
+    <t>Living with asthma</t>
+  </si>
+  <si>
+    <t>Moving to different environments bring new challenges</t>
+  </si>
+  <si>
+    <t>Feeling tired of using inhaler</t>
+  </si>
+  <si>
+    <t>Using inhalers make me inactive</t>
+  </si>
+  <si>
+    <t>Feel bad when dependent to inhalers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Always feeling the need to be careful for </t>
+  </si>
+  <si>
+    <t>Felt healthy for a while so dropped out</t>
+  </si>
+  <si>
+    <t>Felt needy because of illness</t>
+  </si>
+  <si>
+    <t>Increased symptomps after dropping out of treatment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consequence </t>
+  </si>
+  <si>
+    <t>Emotions</t>
+  </si>
+  <si>
+    <t>Felt confident / healthy for a while after treatment</t>
+  </si>
+  <si>
+    <t>Trouble to avoid smoke all the time</t>
+  </si>
+  <si>
+    <t>Perspective of illness detariorated after prescribed with same medicine she got when child</t>
+  </si>
+  <si>
+    <t>Knew asthma is always there, but did not expect it to start over so badly</t>
+  </si>
+  <si>
+    <t>Felt weak regardless of symptoms</t>
+  </si>
+  <si>
+    <t>Felt the need to drop out when realised she is dependent to drugs</t>
+  </si>
+  <si>
+    <t>Surprise?</t>
   </si>
 </sst>
 </file>
@@ -882,20 +1119,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353ADEC9-000A-354D-8FBD-32DD4E097B7B}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="88.375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.375" customWidth="1"/>
-    <col min="5" max="5" width="27.125" customWidth="1"/>
+    <col min="3" max="3" width="88.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -908,8 +1146,14 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -922,8 +1166,14 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -936,8 +1186,14 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -951,10 +1207,13 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -968,10 +1227,13 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -985,10 +1247,13 @@
         <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1002,10 +1267,13 @@
         <v>12</v>
       </c>
       <c r="E7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1019,10 +1287,13 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1035,8 +1306,14 @@
       <c r="D9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1050,10 +1327,13 @@
         <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1067,7 +1347,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1081,7 +1361,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1094,8 +1374,11 @@
       <c r="D13" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1108,8 +1391,14 @@
       <c r="D14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1122,8 +1411,14 @@
       <c r="D15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1136,8 +1431,14 @@
       <c r="D16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1150,8 +1451,14 @@
       <c r="D17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>151</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1164,8 +1471,14 @@
       <c r="D18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1179,7 +1492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1192,8 +1505,14 @@
       <c r="D20" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1206,8 +1525,14 @@
       <c r="D21" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1220,8 +1545,14 @@
       <c r="D22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>151</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1234,8 +1565,14 @@
       <c r="D23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>153</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1248,8 +1585,14 @@
       <c r="D24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>151</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1263,7 +1606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1277,7 +1620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1290,8 +1633,14 @@
       <c r="D27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1305,7 +1654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1319,7 +1668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1333,7 +1682,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1347,7 +1696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1361,7 +1710,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1375,7 +1724,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1388,8 +1737,14 @@
       <c r="D34" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>164</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1402,8 +1757,14 @@
       <c r="D35" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>151</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -1416,8 +1777,14 @@
       <c r="D36" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>153</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1430,8 +1797,14 @@
       <c r="D37" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>151</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1445,7 +1818,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -1458,8 +1831,14 @@
       <c r="D39" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E39" t="s">
+        <v>151</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -1473,7 +1852,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -1486,8 +1865,14 @@
       <c r="D41" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -1500,8 +1885,14 @@
       <c r="D42" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E42" t="s">
+        <v>151</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -1514,8 +1905,14 @@
       <c r="D43" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>151</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -1529,7 +1926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -1542,8 +1939,14 @@
       <c r="D45" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E45" t="s">
+        <v>151</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -1557,7 +1960,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -1570,8 +1973,14 @@
       <c r="D47" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E47" t="s">
+        <v>151</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -1584,8 +1993,14 @@
       <c r="D48" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>175</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -1593,16 +2008,19 @@
         <v>33</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D49" t="s">
         <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>38</v>
       </c>
@@ -1610,13 +2028,19 @@
         <v>33</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D50" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" t="s">
+        <v>143</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>38</v>
       </c>
@@ -1624,16 +2048,19 @@
         <v>33</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D51" t="s">
         <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="F51" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>38</v>
       </c>
@@ -1641,16 +2068,19 @@
         <v>33</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D52" t="s">
         <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="F52" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -1658,16 +2088,19 @@
         <v>33</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D53" t="s">
         <v>5</v>
       </c>
       <c r="E53" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>38</v>
       </c>
@@ -1675,16 +2108,19 @@
         <v>33</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D54" t="s">
         <v>5</v>
       </c>
       <c r="E54" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -1692,13 +2128,19 @@
         <v>33</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D55" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" t="s">
+        <v>184</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -1706,13 +2148,19 @@
         <v>33</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D56" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
+        <v>185</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -1720,10 +2168,16 @@
         <v>33</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E57" t="s">
+        <v>185</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -1731,10 +2185,19 @@
         <v>33</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" t="s">
+        <v>175</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -1742,10 +2205,19 @@
         <v>33</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+      <c r="E59" t="s">
+        <v>185</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>38</v>
       </c>
@@ -1753,10 +2225,19 @@
         <v>33</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" t="s">
+        <v>175</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>38</v>
       </c>
@@ -1764,10 +2245,19 @@
         <v>33</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" t="s">
+        <v>185</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -1775,10 +2265,13 @@
         <v>33</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>38</v>
       </c>
@@ -1786,10 +2279,19 @@
         <v>33</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="D63" t="s">
+        <v>5</v>
+      </c>
+      <c r="E63" t="s">
+        <v>143</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>38</v>
       </c>
@@ -1797,10 +2299,13 @@
         <v>33</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="D64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -1808,10 +2313,10 @@
         <v>33</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -1819,10 +2324,10 @@
         <v>33</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -1830,10 +2335,10 @@
         <v>33</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -1841,10 +2346,10 @@
         <v>33</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -1852,10 +2357,10 @@
         <v>33</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -1863,10 +2368,10 @@
         <v>33</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -1874,10 +2379,10 @@
         <v>33</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>38</v>
       </c>
@@ -1885,10 +2390,10 @@
         <v>33</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>38</v>
       </c>
@@ -1896,27 +2401,374 @@
         <v>33</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>38</v>
       </c>
       <c r="B74" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>38</v>
       </c>
       <c r="B75" t="s">
         <v>35</v>
       </c>
+      <c r="C75" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>38</v>
+      </c>
+      <c r="B76" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>38</v>
+      </c>
+      <c r="B77" t="s">
+        <v>35</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>37</v>
+      </c>
+      <c r="B78" t="s">
+        <v>33</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>37</v>
+      </c>
+      <c r="B79" t="s">
+        <v>33</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>37</v>
+      </c>
+      <c r="B80" t="s">
+        <v>33</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>37</v>
+      </c>
+      <c r="B81" t="s">
+        <v>33</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>37</v>
+      </c>
+      <c r="B82" t="s">
+        <v>33</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>37</v>
+      </c>
+      <c r="B83" t="s">
+        <v>33</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>37</v>
+      </c>
+      <c r="B84" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" t="s">
+        <v>33</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>37</v>
+      </c>
+      <c r="B86" t="s">
+        <v>33</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>37</v>
+      </c>
+      <c r="B87" t="s">
+        <v>33</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>37</v>
+      </c>
+      <c r="B88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>37</v>
+      </c>
+      <c r="B89" t="s">
+        <v>33</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>37</v>
+      </c>
+      <c r="B90" t="s">
+        <v>33</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>37</v>
+      </c>
+      <c r="B91" t="s">
+        <v>33</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>37</v>
+      </c>
+      <c r="B92" t="s">
+        <v>33</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>37</v>
+      </c>
+      <c r="B93" t="s">
+        <v>33</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>37</v>
+      </c>
+      <c r="B94" t="s">
+        <v>33</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>37</v>
+      </c>
+      <c r="B95" t="s">
+        <v>33</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>37</v>
+      </c>
+      <c r="B96" t="s">
+        <v>33</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>37</v>
+      </c>
+      <c r="B97" t="s">
+        <v>33</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>37</v>
+      </c>
+      <c r="B98" t="s">
+        <v>33</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>37</v>
+      </c>
+      <c r="B99" t="s">
+        <v>33</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>39</v>
+      </c>
+      <c r="B100" t="s">
+        <v>33</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>39</v>
+      </c>
+      <c r="B101" t="s">
+        <v>33</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>39</v>
+      </c>
+      <c r="B102" t="s">
+        <v>33</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>39</v>
+      </c>
+      <c r="B103" t="s">
+        <v>33</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>39</v>
+      </c>
+      <c r="B104" t="s">
+        <v>33</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>39</v>
+      </c>
+      <c r="B105" t="s">
+        <v>33</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>39</v>
+      </c>
+      <c r="B106" t="s">
+        <v>33</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D26" xr:uid="{46564A33-8DAE-FB4C-81A7-C0E325B50D95}"/>
+  <autoFilter ref="A1:F106" xr:uid="{64A19340-CFB4-E34D-8BE9-8D8039B16B0D}"/>
   <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Expectation">
       <formula>NOT(ISERROR(SEARCH("Expectation",D1)))</formula>
@@ -1954,9 +2806,9 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1964,7 +2816,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -1972,7 +2824,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1980,7 +2832,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -1988,7 +2840,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2006,21 +2858,21 @@
   <dimension ref="A1:AU9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S31" sqref="S31"/>
+      <selection activeCell="AU9" sqref="AU9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.375" customWidth="1"/>
-    <col min="3" max="47" width="3.375" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="3" max="47" width="3.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>69</v>
       </c>
@@ -2031,7 +2883,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:47" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>70</v>
       </c>
@@ -2171,7 +3023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>71</v>
       </c>
@@ -2308,7 +3160,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>36</v>
       </c>
@@ -2321,13 +3173,13 @@
       <c r="I5" s="4"/>
       <c r="L5" s="6"/>
     </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>37</v>
       </c>
       <c r="Q6" s="5"/>
     </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>38</v>
       </c>
@@ -2340,13 +3192,13 @@
       <c r="W7" s="4"/>
       <c r="AA7" s="6"/>
     </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>39</v>
       </c>
       <c r="Q8" s="5"/>
     </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
work on final deliverables
</commit_message>
<xml_diff>
--- a/assignmentSubmissions/assignment7_coding/coding.xlsx
+++ b/assignmentSubmissions/assignment7_coding/coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burak-inofab/git/ModelingUX/assignmentSubmissions/assignment7_coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A86B2B-1E3F-FF41-9FE4-D8B63B65B965}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3C8159-7F1A-8045-87B0-E9D63D1EE393}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{F4C71E44-69F0-DC4C-BDEB-22E2A60C66CE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{F4C71E44-69F0-DC4C-BDEB-22E2A60C66CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Coding" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Calendar" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coding!$A$1:$F$106</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Coding!$A$1:$F$107</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="216">
   <si>
     <t>Code</t>
   </si>
@@ -609,6 +609,75 @@
   </si>
   <si>
     <t>Surprise?</t>
+  </si>
+  <si>
+    <t>Understanding the illness Is natural and a lot of people have it</t>
+  </si>
+  <si>
+    <t>You should be careful to everything, feeling limited</t>
+  </si>
+  <si>
+    <t>Fear of bee sting because of allergy</t>
+  </si>
+  <si>
+    <t>Cant socialize in smoking environments</t>
+  </si>
+  <si>
+    <t>Forget while rushing in the mornin</t>
+  </si>
+  <si>
+    <t>Put drugs in front of my eyesight</t>
+  </si>
+  <si>
+    <t>Create charts to get motivation</t>
+  </si>
+  <si>
+    <t>Because of staying somewhere else</t>
+  </si>
+  <si>
+    <t>If missed one-two doses it feels easier to dropout</t>
+  </si>
+  <si>
+    <t>Routine change : did not sleep for a deadline</t>
+  </si>
+  <si>
+    <t>I know I will not be completely cuerd but I still use medicine since I know I will be better</t>
+  </si>
+  <si>
+    <t>Excarbation when baby</t>
+  </si>
+  <si>
+    <t>Moving to another city</t>
+  </si>
+  <si>
+    <t>High heat worsens disease</t>
+  </si>
+  <si>
+    <t>Side effects: Weight</t>
+  </si>
+  <si>
+    <t>Side effects: Heart beat</t>
+  </si>
+  <si>
+    <t>Cant socialize because of ilness</t>
+  </si>
+  <si>
+    <t>Family help</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monetary </t>
+  </si>
+  <si>
+    <t>I am my own doctor</t>
+  </si>
+  <si>
+    <t>I am happy with my life</t>
+  </si>
+  <si>
+    <t>Felt better- doctor said so</t>
+  </si>
+  <si>
+    <t>Changed lifestyle, stopped playing sports</t>
   </si>
 </sst>
 </file>
@@ -741,7 +810,174 @@
     <cellStyle name="Behavior" xfId="1" xr:uid="{25E8873D-7408-094E-9CFC-3259DF7FA13A}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="24">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1119,10 +1355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353ADEC9-000A-354D-8FBD-32DD4E097B7B}">
-  <dimension ref="A1:F106"/>
+  <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1227,7 +1463,7 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>184</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>145</v>
@@ -2305,7 +2541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -2315,8 +2551,17 @@
       <c r="C65" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D65" t="s">
+        <v>7</v>
+      </c>
+      <c r="E65" t="s">
+        <v>175</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -2326,8 +2571,17 @@
       <c r="C66" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>7</v>
+      </c>
+      <c r="E66" t="s">
+        <v>175</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -2337,8 +2591,17 @@
       <c r="C67" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>7</v>
+      </c>
+      <c r="E67" t="s">
+        <v>185</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -2348,8 +2611,17 @@
       <c r="C68" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>7</v>
+      </c>
+      <c r="E68" t="s">
+        <v>175</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -2359,8 +2631,14 @@
       <c r="C69" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -2370,8 +2648,17 @@
       <c r="C70" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>5</v>
+      </c>
+      <c r="E70" t="s">
+        <v>151</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -2381,8 +2668,17 @@
       <c r="C71" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D71" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" t="s">
+        <v>153</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>38</v>
       </c>
@@ -2392,8 +2688,17 @@
       <c r="C72" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="D72" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" t="s">
+        <v>153</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>38</v>
       </c>
@@ -2404,7 +2709,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>38</v>
       </c>
@@ -2414,8 +2719,17 @@
       <c r="C74" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D74" t="s">
+        <v>5</v>
+      </c>
+      <c r="E74" t="s">
+        <v>151</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>38</v>
       </c>
@@ -2425,8 +2739,17 @@
       <c r="C75" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D75" t="s">
+        <v>5</v>
+      </c>
+      <c r="E75" t="s">
+        <v>143</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>38</v>
       </c>
@@ -2436,8 +2759,17 @@
       <c r="C76" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D76" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" t="s">
+        <v>151</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -2447,8 +2779,17 @@
       <c r="C77" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D77" t="s">
+        <v>5</v>
+      </c>
+      <c r="E77" t="s">
+        <v>147</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>37</v>
       </c>
@@ -2458,8 +2799,17 @@
       <c r="C78" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>142</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>37</v>
       </c>
@@ -2470,7 +2820,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -2480,8 +2830,14 @@
       <c r="C80" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E80" t="s">
+        <v>175</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>37</v>
       </c>
@@ -2492,7 +2848,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>37</v>
       </c>
@@ -2502,8 +2858,14 @@
       <c r="C82" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E82" t="s">
+        <v>175</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>37</v>
       </c>
@@ -2513,8 +2875,14 @@
       <c r="C83" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E83" t="s">
+        <v>143</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>37</v>
       </c>
@@ -2525,7 +2893,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>37</v>
       </c>
@@ -2535,8 +2903,14 @@
       <c r="C85" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E85" t="s">
+        <v>143</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>37</v>
       </c>
@@ -2546,8 +2920,14 @@
       <c r="C86" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E86" t="s">
+        <v>175</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>37</v>
       </c>
@@ -2558,7 +2938,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>37</v>
       </c>
@@ -2569,7 +2949,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>37</v>
       </c>
@@ -2579,8 +2959,14 @@
       <c r="C89" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E89" t="s">
+        <v>153</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>37</v>
       </c>
@@ -2591,7 +2977,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>37</v>
       </c>
@@ -2602,7 +2988,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>37</v>
       </c>
@@ -2612,8 +2998,11 @@
       <c r="C92" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D92" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>37</v>
       </c>
@@ -2623,8 +3012,17 @@
       <c r="C93" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D93" t="s">
+        <v>7</v>
+      </c>
+      <c r="E93" t="s">
+        <v>143</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>37</v>
       </c>
@@ -2635,7 +3033,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>37</v>
       </c>
@@ -2646,7 +3044,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="96" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>37</v>
       </c>
@@ -2656,8 +3054,14 @@
       <c r="C96" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="E96" t="s">
+        <v>175</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>37</v>
       </c>
@@ -2667,8 +3071,14 @@
       <c r="C97" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E97" t="s">
+        <v>175</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>37</v>
       </c>
@@ -2679,7 +3089,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>37</v>
       </c>
@@ -2689,8 +3099,14 @@
       <c r="C99" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="E99" t="s">
+        <v>175</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -2700,8 +3116,17 @@
       <c r="C100" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" t="s">
+        <v>142</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>39</v>
       </c>
@@ -2712,7 +3137,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>39</v>
       </c>
@@ -2722,8 +3147,14 @@
       <c r="C102" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="E102" t="s">
+        <v>143</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>39</v>
       </c>
@@ -2731,10 +3162,16 @@
         <v>33</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="E103" t="s">
+        <v>184</v>
+      </c>
+      <c r="F103" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>39</v>
       </c>
@@ -2742,10 +3179,16 @@
         <v>33</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="E104" t="s">
+        <v>175</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>39</v>
       </c>
@@ -2753,10 +3196,10 @@
         <v>33</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>39</v>
       </c>
@@ -2764,34 +3207,108 @@
         <v>33</v>
       </c>
       <c r="C106" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>39</v>
+      </c>
+      <c r="B107" t="s">
+        <v>33</v>
+      </c>
+      <c r="C107" s="1" t="s">
         <v>137</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F106" xr:uid="{64A19340-CFB4-E34D-8BE9-8D8039B16B0D}"/>
-  <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Expectation">
+  <autoFilter ref="A1:F107" xr:uid="{64A19340-CFB4-E34D-8BE9-8D8039B16B0D}">
+    <sortState ref="A2:F100">
+      <sortCondition ref="E1:E107"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="D1:D77 D79:D99 D101 D103:D1048576">
+    <cfRule type="containsText" dxfId="23" priority="18" operator="containsText" text="Expectation">
       <formula>NOT(ISERROR(SEARCH("Expectation",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Strategy">
+    <cfRule type="containsText" dxfId="22" priority="21" operator="containsText" text="Strategy">
       <formula>NOT(ISERROR(SEARCH("Strategy",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Concern">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="Concern">
       <formula>NOT(ISERROR(SEARCH("Concern",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Behavior">
+    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="Behavior">
       <formula>NOT(ISERROR(SEARCH("Behavior",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Critical Incident">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="Critical Incident">
       <formula>NOT(ISERROR(SEARCH("Critical Incident",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="After-Diary">
+  <conditionalFormatting sqref="B1:B101 B103:B1048576">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="After-Diary">
       <formula>NOT(ISERROR(SEARCH("After-Diary",B1)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="Pre-Diary">
+      <formula>NOT(ISERROR(SEARCH("Pre-Diary",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D78">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="Expectation">
+      <formula>NOT(ISERROR(SEARCH("Expectation",D78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Strategy">
+      <formula>NOT(ISERROR(SEARCH("Strategy",D78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Concern">
+      <formula>NOT(ISERROR(SEARCH("Concern",D78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Behavior">
+      <formula>NOT(ISERROR(SEARCH("Behavior",D78)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="Critical Incident">
+      <formula>NOT(ISERROR(SEARCH("Critical Incident",D78)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D100">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="Expectation">
+      <formula>NOT(ISERROR(SEARCH("Expectation",D100)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="Strategy">
+      <formula>NOT(ISERROR(SEARCH("Strategy",D100)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Concern">
+      <formula>NOT(ISERROR(SEARCH("Concern",D100)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="Behavior">
+      <formula>NOT(ISERROR(SEARCH("Behavior",D100)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="Critical Incident">
+      <formula>NOT(ISERROR(SEARCH("Critical Incident",D100)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D102">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Expectation">
+      <formula>NOT(ISERROR(SEARCH("Expectation",D102)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Strategy">
+      <formula>NOT(ISERROR(SEARCH("Strategy",D102)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Concern">
+      <formula>NOT(ISERROR(SEARCH("Concern",D102)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Behavior">
+      <formula>NOT(ISERROR(SEARCH("Behavior",D102)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Critical Incident">
+      <formula>NOT(ISERROR(SEARCH("Critical Incident",D102)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B102">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="After-Diary">
+      <formula>NOT(ISERROR(SEARCH("After-Diary",B102)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Pre-Diary">
-      <formula>NOT(ISERROR(SEARCH("Pre-Diary",B1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-Diary",B102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Progress on final deliverables
</commit_message>
<xml_diff>
--- a/assignmentSubmissions/assignment7_coding/coding.xlsx
+++ b/assignmentSubmissions/assignment7_coding/coding.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burak-inofab/git/ModelingUX/assignmentSubmissions/assignment7_coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3C8159-7F1A-8045-87B0-E9D63D1EE393}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0A8324-6B83-DF48-AB60-EF2DA33D9C2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" xr2:uid="{F4C71E44-69F0-DC4C-BDEB-22E2A60C66CE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{F4C71E44-69F0-DC4C-BDEB-22E2A60C66CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Coding" sheetId="1" r:id="rId1"/>
@@ -1355,10 +1355,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353ADEC9-000A-354D-8FBD-32DD4E097B7B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1389,7 +1390,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1449,7 +1450,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1489,7 +1490,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1509,7 +1510,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1529,7 +1530,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1583,7 +1584,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1597,7 +1598,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1614,7 +1615,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1634,7 +1635,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1654,7 +1655,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1674,7 +1675,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1694,7 +1695,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1728,7 +1729,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1748,7 +1749,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1768,7 +1769,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1788,7 +1789,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1808,7 +1809,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1828,7 +1829,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1856,7 +1857,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1876,7 +1877,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1890,7 +1891,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1918,7 +1919,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1960,7 +1961,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1980,7 +1981,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2020,7 +2021,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2040,7 +2041,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2054,7 +2055,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2074,7 +2075,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2088,7 +2089,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -2108,7 +2109,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2148,7 +2149,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="64" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -2162,7 +2163,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -2182,7 +2183,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -2196,7 +2197,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -2216,7 +2217,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -2236,7 +2237,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -2316,7 +2317,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -2356,7 +2357,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -2376,7 +2377,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -2396,7 +2397,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -2433,7 +2434,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -2453,7 +2454,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>38</v>
       </c>
@@ -2473,7 +2474,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>38</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -2527,7 +2528,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>38</v>
       </c>
@@ -2541,7 +2542,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="68" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -2561,7 +2562,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -2581,7 +2582,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -2601,7 +2602,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -2621,7 +2622,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -2658,7 +2659,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -2678,7 +2679,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>38</v>
       </c>
@@ -2698,7 +2699,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>38</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>38</v>
       </c>
@@ -2749,7 +2750,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>38</v>
       </c>
@@ -2769,7 +2770,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -2789,7 +2790,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>37</v>
       </c>
@@ -2809,7 +2810,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>37</v>
       </c>
@@ -2820,7 +2821,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>37</v>
       </c>
@@ -2848,7 +2849,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>37</v>
       </c>
@@ -2882,7 +2883,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>37</v>
       </c>
@@ -2910,7 +2911,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>37</v>
       </c>
@@ -2927,7 +2928,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>37</v>
       </c>
@@ -2938,7 +2939,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>37</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>37</v>
       </c>
@@ -2966,7 +2967,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>37</v>
       </c>
@@ -2977,7 +2978,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>37</v>
       </c>
@@ -2988,7 +2989,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>37</v>
       </c>
@@ -3022,7 +3023,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>37</v>
       </c>
@@ -3033,7 +3034,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>37</v>
       </c>
@@ -3044,7 +3045,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>37</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>37</v>
       </c>
@@ -3078,7 +3079,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>37</v>
       </c>
@@ -3089,7 +3090,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>37</v>
       </c>
@@ -3106,7 +3107,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -3126,7 +3127,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>39</v>
       </c>
@@ -3154,7 +3155,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>39</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>39</v>
       </c>
@@ -3188,7 +3189,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>39</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>39</v>
       </c>
@@ -3210,7 +3211,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>39</v>
       </c>
@@ -3223,6 +3224,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F107" xr:uid="{64A19340-CFB4-E34D-8BE9-8D8039B16B0D}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Drop out reason"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:F100">
       <sortCondition ref="E1:E107"/>
     </sortState>

</xml_diff>

<commit_message>
Add final poster and text deliverables, bye git :)
</commit_message>
<xml_diff>
--- a/assignmentSubmissions/assignment7_coding/coding.xlsx
+++ b/assignmentSubmissions/assignment7_coding/coding.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/burak-inofab/git/ModelingUX/assignmentSubmissions/assignment7_coding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D0A8324-6B83-DF48-AB60-EF2DA33D9C2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F21365-C943-5541-BA7B-BAD9442F1E41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{F4C71E44-69F0-DC4C-BDEB-22E2A60C66CE}"/>
   </bookViews>
@@ -1355,11 +1355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{353ADEC9-000A-354D-8FBD-32DD4E097B7B}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1390,7 +1389,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1490,7 +1489,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1510,7 +1509,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1530,7 +1529,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1550,7 +1549,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1570,7 +1569,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1584,7 +1583,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -1598,7 +1597,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -1615,7 +1614,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1635,7 +1634,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1655,7 +1654,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -1675,7 +1674,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1695,7 +1694,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1715,7 +1714,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1729,7 +1728,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1749,7 +1748,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -1769,7 +1768,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1789,7 +1788,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -1809,7 +1808,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>36</v>
       </c>
@@ -1829,7 +1828,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>36</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -1857,7 +1856,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -1877,7 +1876,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -1891,7 +1890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -1905,7 +1904,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1919,7 +1918,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1933,7 +1932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -1947,7 +1946,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1961,7 +1960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1981,7 +1980,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -2001,7 +2000,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2021,7 +2020,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2041,7 +2040,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2055,7 +2054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2075,7 +2074,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2089,7 +2088,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -2109,7 +2108,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>36</v>
       </c>
@@ -2129,7 +2128,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -2149,7 +2148,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="64" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>36</v>
       </c>
@@ -2163,7 +2162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>36</v>
       </c>
@@ -2183,7 +2182,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -2197,7 +2196,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -2217,7 +2216,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>38</v>
       </c>
@@ -2237,7 +2236,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -2317,7 +2316,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -2357,7 +2356,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>38</v>
       </c>
@@ -2377,7 +2376,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>38</v>
       </c>
@@ -2397,7 +2396,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>38</v>
       </c>
@@ -2414,7 +2413,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>38</v>
       </c>
@@ -2434,7 +2433,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -2454,7 +2453,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>38</v>
       </c>
@@ -2474,7 +2473,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>38</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>38</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>38</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="68" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>38</v>
       </c>
@@ -2562,7 +2561,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>38</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>38</v>
       </c>
@@ -2602,7 +2601,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>38</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>38</v>
       </c>
@@ -2639,7 +2638,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>38</v>
       </c>
@@ -2659,7 +2658,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>38</v>
       </c>
@@ -2679,7 +2678,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>38</v>
       </c>
@@ -2699,7 +2698,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>38</v>
       </c>
@@ -2710,7 +2709,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>38</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>38</v>
       </c>
@@ -2770,7 +2769,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>38</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>37</v>
       </c>
@@ -2810,7 +2809,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>37</v>
       </c>
@@ -2821,7 +2820,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>37</v>
       </c>
@@ -2838,7 +2837,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>37</v>
       </c>
@@ -2849,7 +2848,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>37</v>
       </c>
@@ -2883,7 +2882,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>37</v>
       </c>
@@ -2911,7 +2910,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>37</v>
       </c>
@@ -2928,7 +2927,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>37</v>
       </c>
@@ -2939,7 +2938,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>37</v>
       </c>
@@ -2950,7 +2949,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>37</v>
       </c>
@@ -2967,7 +2966,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>37</v>
       </c>
@@ -2978,7 +2977,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>37</v>
       </c>
@@ -2989,7 +2988,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>37</v>
       </c>
@@ -3023,7 +3022,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>37</v>
       </c>
@@ -3034,7 +3033,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>37</v>
       </c>
@@ -3045,7 +3044,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>37</v>
       </c>
@@ -3062,7 +3061,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="51" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>37</v>
       </c>
@@ -3079,7 +3078,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>37</v>
       </c>
@@ -3090,7 +3089,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>37</v>
       </c>
@@ -3107,7 +3106,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>39</v>
       </c>
@@ -3127,7 +3126,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>39</v>
       </c>
@@ -3155,7 +3154,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>39</v>
       </c>
@@ -3172,7 +3171,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="34" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>39</v>
       </c>
@@ -3189,7 +3188,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>39</v>
       </c>
@@ -3200,7 +3199,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>39</v>
       </c>
@@ -3211,7 +3210,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>39</v>
       </c>
@@ -3224,12 +3223,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F107" xr:uid="{64A19340-CFB4-E34D-8BE9-8D8039B16B0D}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Drop out reason"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A2:F100">
+    <sortState ref="A48:F104">
       <sortCondition ref="E1:E107"/>
     </sortState>
   </autoFilter>

</xml_diff>